<commit_message>
add extraction parameters to Metabolights chromatography template
</commit_message>
<xml_diff>
--- a/background information/MetaboLights/metabolights.xlsx
+++ b/background information/MetaboLights/metabolights.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\sciebo - Eggels, Stella (s.eggels@fz-juelich.de)@fz-juelich.sciebo.de\SE\DataPLANT\SWATE templates meetings\Repository requirements etc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\background information\MetaboLights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CE4752-1C32-4604-9254-663453A81ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B5C16C-4D52-4B77-88E7-E57FA53180D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0096593A-FF03-4B73-8EDB-D9A655C6C356}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0096593A-FF03-4B73-8EDB-D9A655C6C356}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>NMR</t>
   </si>
@@ -171,9 +170,6 @@
     <t>Sample name</t>
   </si>
   <si>
-    <t>Swate template</t>
-  </si>
-  <si>
     <t>protocol type</t>
   </si>
   <si>
@@ -193,6 +189,24 @@
   </si>
   <si>
     <t>https://www.ebi.ac.uk/metabolights/editor/guides/Assay/Assay_overview</t>
+  </si>
+  <si>
+    <t>Swate template: Chromatography</t>
+  </si>
+  <si>
+    <t>Swate template: Mass spectrometry</t>
+  </si>
+  <si>
+    <t>protocol type, protocol ref</t>
+  </si>
+  <si>
+    <t>solvent extraction</t>
+  </si>
+  <si>
+    <t>derivatisation</t>
+  </si>
+  <si>
+    <t>last updated: 23.4.24</t>
   </si>
 </sst>
 </file>
@@ -269,14 +283,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -616,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED24E31-6044-4BED-9FCF-483D3ECC09C5}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,12 +640,12 @@
     <col min="1" max="1" width="60.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="29.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -644,10 +657,18 @@
         <v>41</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>26</v>
       </c>
@@ -658,7 +679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -669,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -679,16 +700,22 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -699,46 +726,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>10</v>
       </c>
@@ -749,10 +776,10 @@
         <v>30</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>11</v>
       </c>
@@ -766,49 +793,49 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>15</v>
       </c>
@@ -822,15 +849,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>17</v>
       </c>
@@ -840,11 +867,11 @@
       <c r="D26" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F26" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -854,11 +881,11 @@
       <c r="D27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>19</v>
       </c>
@@ -868,66 +895,66 @@
       <c r="D28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C31" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C33" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F33" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>20</v>
       </c>
@@ -938,7 +965,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>21</v>
       </c>
@@ -949,7 +976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>22</v>
       </c>
@@ -960,7 +987,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>23</v>
       </c>
@@ -971,7 +998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>24</v>
       </c>
@@ -982,7 +1009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
move MIAPPE and MetaboLights templates to subfolders
</commit_message>
<xml_diff>
--- a/background information/MetaboLights/metabolights.xlsx
+++ b/background information/MetaboLights/metabolights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\background information\MetaboLights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B5C16C-4D52-4B77-88E7-E57FA53180D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638B75B5-1A15-4869-A453-63331DA4B203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0096593A-FF03-4B73-8EDB-D9A655C6C356}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
   <si>
     <t>NMR</t>
   </si>
@@ -206,33 +206,50 @@
     <t>derivatisation</t>
   </si>
   <si>
-    <t>last updated: 23.4.24</t>
+    <t>last updated: 24.4.24</t>
+  </si>
+  <si>
+    <t>NMR sample tube</t>
+  </si>
+  <si>
+    <t>NMR solvent</t>
+  </si>
+  <si>
+    <t>sample pH</t>
+  </si>
+  <si>
+    <t>sample temperature</t>
+  </si>
+  <si>
+    <t>Swate template: NMR sample</t>
+  </si>
+  <si>
+    <t>Swate template: NMR spectroscopy</t>
+  </si>
+  <si>
+    <t>NMR instrument</t>
+  </si>
+  <si>
+    <t>Number of scans</t>
+  </si>
+  <si>
+    <t>Pulse sequence name</t>
+  </si>
+  <si>
+    <t>magnetic field strength</t>
+  </si>
+  <si>
+    <t>sample</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,8 +261,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="6"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -283,13 +300,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -629,394 +645,443 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED24E31-6044-4BED-9FCF-483D3ECC09C5}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="29.5546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="29.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="29.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="E18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="F18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="G18" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="F19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="G19" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="G20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="F21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="G21" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="F22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="G22" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="F23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="G23" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="E26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="F26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="H26" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="E27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="F27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="H27" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="E28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="F28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="H28" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C29" s="5" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="F29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="H29" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C30" s="5" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="F30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="H30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="5" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="F31" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="H31" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="5" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="F32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C33" s="5" t="s">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="F33" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="H33" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D37" t="s">
+      <c r="F37" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C41" t="s">
+      <c r="E41" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D41" t="s">
+      <c r="F41" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>